<commit_message>
RED9 - Push ATTR     reset - added multiplier value to blend from current to default    get_default - few tweaks MRSANIMATE - Lots of work. New sections > hold,tween
</commit_message>
<xml_diff>
--- a/mayaTools/Red9/Codebase_Tracker.xlsx
+++ b/mayaTools/Red9/Codebase_Tracker.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="292">
   <si>
     <t>Module</t>
   </si>
@@ -865,6 +865,33 @@
   </si>
   <si>
     <t>!!</t>
+  </si>
+  <si>
+    <t>Added direct exposure of the animPointCloud to the Pro_MetaRig so that we can use it to transpose world space on the fly</t>
+  </si>
+  <si>
+    <t>this isn't yet exposed except in code but is a really key function to allow us to change data on the fly without it effecting the rigs pose</t>
+  </si>
+  <si>
+    <t>anim_point_cloud  - code</t>
+  </si>
+  <si>
+    <t>switch_attr_compensated - code</t>
+  </si>
+  <si>
+    <t>a wrapper over the anim_point_cloud, allowing an attribute on a node to be changed whilst compensating for that change in the rigs transforms</t>
+  </si>
+  <si>
+    <t>this will eventually be exposed to allow us to change Parent spaces on the fly, both static and over time</t>
+  </si>
+  <si>
+    <t>ik_fk_match, fk_ik_match</t>
+  </si>
+  <si>
+    <t>new timerange flag added to allow us to directly pass in the timerange to process</t>
+  </si>
+  <si>
+    <t>previously time was just a bool which triggered a get of the current timeline bounds only</t>
   </si>
 </sst>
 </file>
@@ -1060,7 +1087,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1407,11 +1434,20 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="4" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1726,10 +1762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:M69"/>
+  <dimension ref="A2:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1748,17 +1784,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="21">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="117" t="s">
         <v>137</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
     </row>
     <row r="3" spans="1:13" ht="15.6" customHeight="1"/>
     <row r="4" spans="1:13" s="2" customFormat="1" ht="24" customHeight="1">
@@ -2610,7 +2646,7 @@
       <c r="I39" s="31"/>
       <c r="J39" s="68"/>
     </row>
-    <row r="40" spans="2:10" ht="15.75">
+    <row r="40" spans="2:10" ht="21" customHeight="1">
       <c r="B40" s="26" t="s">
         <v>16</v>
       </c>
@@ -2743,231 +2779,252 @@
       </c>
       <c r="J44" s="112"/>
     </row>
-    <row r="45" spans="2:10" ht="30" customHeight="1">
-      <c r="C45" s="52"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="2:10" ht="60">
-      <c r="B46" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C46" s="49" t="s">
+    <row r="45" spans="2:10" ht="45">
+      <c r="B45" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C45" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="E45" s="75">
+        <v>43154</v>
+      </c>
+      <c r="F45" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G45" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>283</v>
+      </c>
+      <c r="I45" s="31" t="s">
+        <v>284</v>
+      </c>
+      <c r="J45" s="120"/>
+    </row>
+    <row r="46" spans="2:10" ht="45">
+      <c r="B46" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C46" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="E46" s="75">
+        <v>43154</v>
+      </c>
+      <c r="F46" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="H46" s="31" t="s">
+        <v>287</v>
+      </c>
+      <c r="I46" s="31" t="s">
+        <v>288</v>
+      </c>
+      <c r="J46" s="120"/>
+    </row>
+    <row r="47" spans="2:10" ht="30">
+      <c r="B47" s="118" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="119" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="119" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="75">
+        <v>43154</v>
+      </c>
+      <c r="F47" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="G47" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="H47" s="31" t="s">
+        <v>290</v>
+      </c>
+      <c r="I47" s="31" t="s">
+        <v>291</v>
+      </c>
+      <c r="J47" s="120"/>
+    </row>
+    <row r="48" spans="2:10" ht="30" customHeight="1">
+      <c r="C48" s="52"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="11"/>
+    </row>
+    <row r="49" spans="1:10" ht="60">
+      <c r="B49" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C49" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="20" t="s">
+      <c r="D49" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E46" s="21">
+      <c r="E49" s="21">
         <v>42734</v>
       </c>
-      <c r="F46" s="22" t="s">
+      <c r="F49" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G46" s="23" t="s">
+      <c r="G49" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="H46" s="24" t="s">
+      <c r="H49" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="I46" s="24" t="s">
+      <c r="I49" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="J46" s="67"/>
-    </row>
-    <row r="47" spans="2:10" ht="45">
-      <c r="B47" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C47" s="50" t="s">
+      <c r="J49" s="67"/>
+    </row>
+    <row r="50" spans="1:10" ht="45">
+      <c r="B50" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C50" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="35" t="s">
+      <c r="D50" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E47" s="36">
+      <c r="E50" s="36">
         <v>42740</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F50" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G47" s="40" t="s">
+      <c r="G50" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="H47" s="38" t="s">
+      <c r="H50" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="I47" s="35"/>
-      <c r="J47" s="66"/>
-    </row>
-    <row r="48" spans="2:10" ht="45">
-      <c r="B48" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="49" t="s">
+      <c r="I50" s="35"/>
+      <c r="J50" s="66"/>
+    </row>
+    <row r="51" spans="1:10" ht="45">
+      <c r="B51" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D51" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E51" s="21">
         <v>42745</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F51" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G48" s="23" t="s">
+      <c r="G51" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="H48" s="24" t="s">
+      <c r="H51" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I48" s="20" t="s">
+      <c r="I51" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="J48" s="67"/>
-    </row>
-    <row r="49" spans="1:10" ht="45">
-      <c r="B49" s="79" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="80" t="s">
+      <c r="J51" s="67"/>
+    </row>
+    <row r="52" spans="1:10" ht="45">
+      <c r="B52" s="79" t="s">
+        <v>16</v>
+      </c>
+      <c r="C52" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="D49" s="83" t="s">
+      <c r="D52" s="83" t="s">
         <v>13</v>
       </c>
-      <c r="E49" s="81">
+      <c r="E52" s="81">
         <v>42811</v>
       </c>
-      <c r="F49" s="13" t="s">
+      <c r="F52" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G49" s="46" t="s">
+      <c r="G52" s="46" t="s">
         <v>151</v>
       </c>
-      <c r="H49" s="84" t="s">
+      <c r="H52" s="84" t="s">
         <v>152</v>
       </c>
-      <c r="I49" s="83" t="s">
+      <c r="I52" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="J49" s="82"/>
-    </row>
-    <row r="50" spans="1:10" ht="45">
-      <c r="B50" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="73" t="s">
+      <c r="J52" s="82"/>
+    </row>
+    <row r="53" spans="1:10" ht="45">
+      <c r="B53" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C53" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D50" s="87" t="s">
+      <c r="D53" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="88">
+      <c r="E53" s="88">
         <v>42817</v>
       </c>
-      <c r="F50" s="89" t="s">
+      <c r="F53" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="G50" s="30" t="s">
+      <c r="G53" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H50" s="78" t="s">
+      <c r="H53" s="78" t="s">
         <v>161</v>
       </c>
-      <c r="I50" s="78" t="s">
+      <c r="I53" s="78" t="s">
         <v>162</v>
       </c>
-      <c r="J50" s="90"/>
-    </row>
-    <row r="51" spans="1:10" ht="30">
-      <c r="B51" s="86" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="73" t="s">
+      <c r="J53" s="90"/>
+    </row>
+    <row r="54" spans="1:10" ht="30">
+      <c r="B54" s="86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="87" t="s">
+      <c r="D54" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="88">
+      <c r="E54" s="88">
         <v>43110</v>
       </c>
-      <c r="F51" s="89" t="s">
+      <c r="F54" s="89" t="s">
         <v>98</v>
       </c>
-      <c r="G51" s="30" t="s">
+      <c r="G54" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="H51" s="78" t="s">
+      <c r="H54" s="78" t="s">
         <v>273</v>
       </c>
-      <c r="I51" s="78" t="s">
+      <c r="I54" s="78" t="s">
         <v>274</v>
       </c>
-      <c r="J51" s="90"/>
-    </row>
-    <row r="52" spans="1:10" ht="30" customHeight="1">
-      <c r="C52" s="52"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="11"/>
-    </row>
-    <row r="53" spans="1:10" ht="30">
-      <c r="B53" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C53" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="D53" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="E53" s="21">
-        <v>42745</v>
-      </c>
-      <c r="F53" s="22" t="s">
-        <v>107</v>
-      </c>
-      <c r="G53" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="H53" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="I53" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="J53" s="67"/>
-    </row>
-    <row r="54" spans="1:10" ht="60">
-      <c r="B54" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C54" s="73" t="s">
-        <v>119</v>
-      </c>
-      <c r="D54" s="87" t="s">
-        <v>187</v>
-      </c>
-      <c r="E54" s="75">
-        <v>43110</v>
-      </c>
-      <c r="F54" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="G54" s="30" t="s">
-        <v>270</v>
-      </c>
-      <c r="H54" s="78" t="s">
-        <v>271</v>
-      </c>
-      <c r="I54" s="78" t="s">
-        <v>272</v>
-      </c>
-      <c r="J54" s="77"/>
+      <c r="J54" s="90"/>
     </row>
     <row r="55" spans="1:10" ht="30" customHeight="1">
       <c r="C55" s="52"/>
@@ -2975,314 +3032,374 @@
       <c r="G55" s="7"/>
       <c r="H55" s="11"/>
     </row>
-    <row r="56" spans="1:10" ht="45">
+    <row r="56" spans="1:10" ht="30">
       <c r="B56" s="19" t="s">
         <v>16</v>
       </c>
       <c r="C56" s="49" t="s">
-        <v>18</v>
+        <v>119</v>
       </c>
       <c r="D56" s="20" t="s">
-        <v>14</v>
+        <v>120</v>
       </c>
       <c r="E56" s="21">
-        <v>42734</v>
+        <v>42745</v>
       </c>
       <c r="F56" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G56" s="23"/>
+      <c r="G56" s="23" t="s">
+        <v>121</v>
+      </c>
       <c r="H56" s="24" t="s">
+        <v>122</v>
+      </c>
+      <c r="I56" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="J56" s="67"/>
+    </row>
+    <row r="57" spans="1:10" ht="60">
+      <c r="B57" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C57" s="73" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="87" t="s">
+        <v>187</v>
+      </c>
+      <c r="E57" s="75">
+        <v>43110</v>
+      </c>
+      <c r="F57" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="G57" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="H57" s="78" t="s">
+        <v>271</v>
+      </c>
+      <c r="I57" s="78" t="s">
+        <v>272</v>
+      </c>
+      <c r="J57" s="77"/>
+    </row>
+    <row r="58" spans="1:10" ht="30" customHeight="1">
+      <c r="C58" s="52"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="11"/>
+    </row>
+    <row r="59" spans="1:10" ht="45">
+      <c r="B59" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C59" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E59" s="21">
+        <v>42734</v>
+      </c>
+      <c r="F59" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="G59" s="23"/>
+      <c r="H59" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I56" s="20"/>
-      <c r="J56" s="67"/>
-    </row>
-    <row r="57" spans="1:10" ht="45">
-      <c r="B57" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57" s="49" t="s">
+      <c r="I59" s="20"/>
+      <c r="J59" s="67"/>
+    </row>
+    <row r="60" spans="1:10" ht="45">
+      <c r="B60" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C60" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D60" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E57" s="21">
+      <c r="E60" s="21">
         <v>42734</v>
       </c>
-      <c r="F57" s="93" t="s">
+      <c r="F60" s="93" t="s">
         <v>107</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="H57" s="24" t="s">
+      <c r="G60" s="23"/>
+      <c r="H60" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="I57" s="20"/>
-      <c r="J57" s="67"/>
-    </row>
-    <row r="58" spans="1:10" ht="75">
-      <c r="A58" s="115" t="s">
+      <c r="I60" s="20"/>
+      <c r="J60" s="67"/>
+    </row>
+    <row r="61" spans="1:10" ht="75">
+      <c r="A61" s="115" t="s">
         <v>282</v>
       </c>
-      <c r="B58" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="117" t="s">
+      <c r="B61" s="72" t="s">
+        <v>16</v>
+      </c>
+      <c r="C61" s="116" t="s">
         <v>18</v>
       </c>
-      <c r="D58" s="74" t="s">
+      <c r="D61" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="E58" s="75">
+      <c r="E61" s="75">
         <v>43110</v>
       </c>
-      <c r="F58" s="113" t="s">
+      <c r="F61" s="113" t="s">
         <v>97</v>
       </c>
-      <c r="G58" s="76" t="s">
+      <c r="G61" s="76" t="s">
         <v>279</v>
       </c>
-      <c r="H58" s="114" t="s">
+      <c r="H61" s="114" t="s">
         <v>280</v>
       </c>
-      <c r="I58" s="74" t="s">
+      <c r="I61" s="74" t="s">
         <v>281</v>
       </c>
-      <c r="J58" s="77"/>
-    </row>
-    <row r="59" spans="1:10" ht="30" customHeight="1">
-      <c r="C59" s="52"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="11"/>
-    </row>
-    <row r="60" spans="1:10" ht="60">
-      <c r="B60" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C60" s="55" t="s">
+      <c r="J61" s="77"/>
+    </row>
+    <row r="62" spans="1:10" ht="30" customHeight="1">
+      <c r="C62" s="52"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="1:10" ht="60">
+      <c r="B63" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C63" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="33"/>
-      <c r="E60" s="44">
+      <c r="D63" s="33"/>
+      <c r="E63" s="44">
         <v>42709</v>
       </c>
-      <c r="F60" s="45" t="s">
+      <c r="F63" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="G60" s="46"/>
-      <c r="H60" s="47" t="s">
+      <c r="G63" s="46"/>
+      <c r="H63" s="47" t="s">
         <v>21</v>
       </c>
-      <c r="I60" s="47" t="s">
+      <c r="I63" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="J60" s="70" t="s">
+      <c r="J63" s="70" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="45">
-      <c r="B61" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="49" t="s">
+    <row r="64" spans="1:10" ht="45">
+      <c r="B64" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="20"/>
-      <c r="E61" s="21">
+      <c r="D64" s="20"/>
+      <c r="E64" s="21">
         <v>42749</v>
       </c>
-      <c r="F61" s="22" t="s">
+      <c r="F64" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="G61" s="20"/>
-      <c r="H61" s="24" t="s">
+      <c r="G64" s="20"/>
+      <c r="H64" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="I61" s="24" t="s">
+      <c r="I64" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="J61" s="67"/>
-    </row>
-    <row r="62" spans="1:10" ht="30">
-      <c r="B62" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="50" t="s">
+      <c r="J64" s="67"/>
+    </row>
+    <row r="65" spans="2:10" ht="30">
+      <c r="B65" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C65" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="35"/>
-      <c r="E62" s="36">
+      <c r="D65" s="35"/>
+      <c r="E65" s="36">
         <v>42809</v>
       </c>
-      <c r="F62" s="37" t="s">
+      <c r="F65" s="37" t="s">
         <v>97</v>
       </c>
-      <c r="G62" s="40"/>
-      <c r="H62" s="38" t="s">
+      <c r="G65" s="40"/>
+      <c r="H65" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="I62" s="38" t="s">
+      <c r="I65" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="J62" s="66"/>
-    </row>
-    <row r="64" spans="1:10" ht="28.5" customHeight="1">
-      <c r="B64" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="54" t="s">
+      <c r="J65" s="66"/>
+    </row>
+    <row r="67" spans="2:10" ht="28.5" customHeight="1">
+      <c r="B67" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="54" t="s">
         <v>176</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D67" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="E64" s="18">
+      <c r="E67" s="18">
         <v>42781</v>
       </c>
-      <c r="F64" s="13" t="s">
+      <c r="F67" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="G64" s="14" t="s">
+      <c r="G67" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="H64" s="15" t="s">
+      <c r="H67" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="I64" s="14"/>
-      <c r="J64" s="69"/>
-    </row>
-    <row r="65" spans="2:10" ht="30">
-      <c r="B65" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="55" t="s">
+      <c r="I67" s="14"/>
+      <c r="J67" s="69"/>
+    </row>
+    <row r="68" spans="2:10" ht="30">
+      <c r="B68" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C68" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D65" s="33" t="s">
+      <c r="D68" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="E65" s="44">
+      <c r="E68" s="44">
         <v>42468</v>
       </c>
-      <c r="F65" s="45" t="s">
+      <c r="F68" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G65" s="46" t="s">
+      <c r="G68" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="H65" s="47" t="s">
+      <c r="H68" s="47" t="s">
         <v>178</v>
       </c>
-      <c r="I65" s="47"/>
-      <c r="J65" s="70"/>
-    </row>
-    <row r="66" spans="2:10" ht="30">
-      <c r="B66" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" s="55" t="s">
+      <c r="I68" s="47"/>
+      <c r="J68" s="70"/>
+    </row>
+    <row r="69" spans="2:10" ht="30">
+      <c r="B69" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C69" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D66" s="33" t="s">
+      <c r="D69" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="E66" s="44">
+      <c r="E69" s="44">
         <v>42451</v>
       </c>
-      <c r="F66" s="45" t="s">
+      <c r="F69" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G66" s="46" t="s">
+      <c r="G69" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="H66" s="47" t="s">
+      <c r="H69" s="47" t="s">
         <v>180</v>
       </c>
-      <c r="I66" s="47"/>
-      <c r="J66" s="70"/>
-    </row>
-    <row r="67" spans="2:10" ht="45">
-      <c r="B67" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="C67" s="55" t="s">
+      <c r="I69" s="47"/>
+      <c r="J69" s="70"/>
+    </row>
+    <row r="70" spans="2:10" ht="45">
+      <c r="B70" s="43" t="s">
+        <v>16</v>
+      </c>
+      <c r="C70" s="55" t="s">
         <v>176</v>
       </c>
-      <c r="D67" s="33" t="s">
+      <c r="D70" s="33" t="s">
         <v>181</v>
       </c>
-      <c r="E67" s="44">
+      <c r="E70" s="44">
         <v>42488</v>
       </c>
-      <c r="F67" s="45" t="s">
+      <c r="F70" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="G67" s="46" t="s">
+      <c r="G70" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="H67" s="47" t="s">
+      <c r="H70" s="47" t="s">
         <v>182</v>
       </c>
-      <c r="I67" s="47" t="s">
+      <c r="I70" s="47" t="s">
         <v>183</v>
       </c>
-      <c r="J67" s="70"/>
-    </row>
-    <row r="68" spans="2:10" ht="30">
-      <c r="B68" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C68" s="51" t="s">
+      <c r="J70" s="70"/>
+    </row>
+    <row r="71" spans="2:10" ht="30">
+      <c r="B71" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C71" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="D68" s="27" t="s">
+      <c r="D71" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="E68" s="28">
+      <c r="E71" s="28">
         <v>43013</v>
       </c>
-      <c r="F68" s="29" t="s">
+      <c r="F71" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G68" s="30" t="s">
+      <c r="G71" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="H68" s="31" t="s">
+      <c r="H71" s="31" t="s">
         <v>224</v>
       </c>
-      <c r="I68" s="31" t="s">
+      <c r="I71" s="31" t="s">
         <v>225</v>
       </c>
-      <c r="J68" s="68"/>
-    </row>
-    <row r="69" spans="2:10" ht="30">
-      <c r="B69" s="26" t="s">
-        <v>16</v>
-      </c>
-      <c r="C69" s="51" t="s">
+      <c r="J71" s="68"/>
+    </row>
+    <row r="72" spans="2:10" ht="30">
+      <c r="B72" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="D69" s="27" t="s">
+      <c r="D72" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="E69" s="28">
+      <c r="E72" s="28">
         <v>43047</v>
       </c>
-      <c r="F69" s="29" t="s">
+      <c r="F72" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="G69" s="30" t="s">
+      <c r="G72" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="H69" s="31" t="s">
+      <c r="H72" s="31" t="s">
         <v>248</v>
       </c>
-      <c r="I69" s="31" t="s">
+      <c r="I72" s="31" t="s">
         <v>249</v>
       </c>
-      <c r="J69" s="68"/>
+      <c r="J72" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3317,17 +3434,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="117" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
     </row>
     <row r="4" spans="2:13" s="8" customFormat="1">
       <c r="B4" s="3" t="s">

</xml_diff>